<commit_message>
Fix worksheets not calling global named ranges created by another worksheet.
</commit_message>
<xml_diff>
--- a/ClosedXML/ClosedXML/ClosedXML_Tests/Resource/Examples/ConditionalFormatting/CFStartsWith.xlsx
+++ b/ClosedXML/ClosedXML/ClosedXML_Tests/Resource/Examples/ConditionalFormatting/CFStartsWith.xlsx
@@ -103,7 +103,20 @@
           <x:bgColor rgb="FFFF0000"/>
         </x:patternFill>
       </x:fill>
-      <x:border/>
+      <x:border>
+        <x:left style="thick">
+          <x:color rgb="FF0000FF"/>
+        </x:left>
+        <x:right style="thick">
+          <x:color rgb="FF0000FF"/>
+        </x:right>
+        <x:top style="thick">
+          <x:color rgb="FF0000FF"/>
+        </x:top>
+        <x:bottom style="thick">
+          <x:color rgb="FF0000FF"/>
+        </x:bottom>
+      </x:border>
     </x:dxf>
     <x:dxf>
       <x:font>
@@ -115,7 +128,20 @@
           <x:bgColor rgb="FFFF0000"/>
         </x:patternFill>
       </x:fill>
-      <x:border/>
+      <x:border>
+        <x:left style="thick">
+          <x:color rgb="FF0000FF"/>
+        </x:left>
+        <x:right style="thick">
+          <x:color rgb="FF0000FF"/>
+        </x:right>
+        <x:top style="thick">
+          <x:color rgb="FF0000FF"/>
+        </x:top>
+        <x:bottom style="thick">
+          <x:color rgb="FF0000FF"/>
+        </x:bottom>
+      </x:border>
     </x:dxf>
   </x:dxfs>
 </x:styleSheet>

</xml_diff>